<commit_message>
Sprint 2 completion and Sprint 3 planning
</commit_message>
<xml_diff>
--- a/TeamBravo Report rev 1.xlsx
+++ b/TeamBravo Report rev 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chauh\Documents\SSW 555\ssw_555_scrum_master_documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C597B9-C4C0-429E-9D97-0998A5514860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048573FA-DD04-4687-96EF-F1223D523A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="332">
   <si>
     <t>Done</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -513,30 +513,9 @@
     <t>End Customer Service API</t>
   </si>
   <si>
-    <t>End-Customer: Create REST API Framework using Swagger</t>
-  </si>
-  <si>
-    <t>Customer Agreement view API</t>
-  </si>
-  <si>
-    <t>Customer Agreement Confirmation API</t>
-  </si>
-  <si>
-    <t>Customer Work Tracking API</t>
-  </si>
-  <si>
     <t>Sales Service API</t>
   </si>
   <si>
-    <t>S5-56</t>
-  </si>
-  <si>
-    <t>S5-57</t>
-  </si>
-  <si>
-    <t>S5-58</t>
-  </si>
-  <si>
     <t>S5-50</t>
   </si>
   <si>
@@ -804,9 +783,6 @@
     <t>S5-93</t>
   </si>
   <si>
-    <t>Setup AWS EC2 instance for Sales Service</t>
-  </si>
-  <si>
     <t>S5-79</t>
   </si>
   <si>
@@ -832,9 +808,6 @@
   </si>
   <si>
     <t>As a UI Designer, I want to create a visually appealing homepage that provides easy access to all the key features of the website, so that users can navigate the site with ease.</t>
-  </si>
-  <si>
-    <t>As a developer, create a REST API Frame for End Customer Service APIS so that structure can be used to create service logic over it</t>
   </si>
   <si>
     <t>As a requirement engineer, I want to identify the key features and functionalities required between each stakeholder which will include maker-checker rules, inter-relationships between stakeholders, and the impact of transition. Specify the data and analytics involved, so that I can develop a prototype that meets their needs and expectations.</t>
@@ -1074,6 +1047,312 @@
         <family val="2"/>
       </rPr>
       <t>ommit after every change rather than commiting all at once especially towards end of sprint</t>
+    </r>
+  </si>
+  <si>
+    <t>S5-98</t>
+  </si>
+  <si>
+    <t>As a developer, I want to create a customer installation tracking API so that customer can track installation using the response returned by the API.</t>
+  </si>
+  <si>
+    <t>End-Customer: Customer Installation Tracking Service API</t>
+  </si>
+  <si>
+    <t>End-Customer: Customer Installation Tracking UI</t>
+  </si>
+  <si>
+    <t>S5-97</t>
+  </si>
+  <si>
+    <t>As a UI Designer, I want to create a customer installation tracking page so that customers can track installation when page is opened</t>
+  </si>
+  <si>
+    <t>As a developer, I want to integrate Database with service using ORM so that all service can persist into AWS RDS database.</t>
+  </si>
+  <si>
+    <t>S5-100</t>
+  </si>
+  <si>
+    <t>Database Integration with all Service</t>
+  </si>
+  <si>
+    <t>S5-94</t>
+  </si>
+  <si>
+    <t>Sales: Customer onboarding UI and Services Integration and Testing</t>
+  </si>
+  <si>
+    <t>As a Developer and Tester, I want to integrate Customer onboarding UI and Service and perform Testing so that I can verify there no bugs in the flow.</t>
+  </si>
+  <si>
+    <t>Sales: Customer Agreement View Unit Test Case and Smoke Test</t>
+  </si>
+  <si>
+    <t>S5-96</t>
+  </si>
+  <si>
+    <t>As a Developer and Tester, I want to integrate Customer agreement view UI and Service and perform Testing so that I can verify there no bugs in the flow.</t>
+  </si>
+  <si>
+    <t>Setup AWS EC2 instance and AWS CodeDeploy for Sales Service</t>
+  </si>
+  <si>
+    <t>S5-102</t>
+  </si>
+  <si>
+    <t>Create Customer Installation API</t>
+  </si>
+  <si>
+    <t>S5-103</t>
+  </si>
+  <si>
+    <t>Dev Test Customer Installation Tracking API</t>
+  </si>
+  <si>
+    <t>S5-106</t>
+  </si>
+  <si>
+    <t>Create Customer Installation UI</t>
+  </si>
+  <si>
+    <t>S5-107</t>
+  </si>
+  <si>
+    <t>Dev test UI</t>
+  </si>
+  <si>
+    <t>S5-108</t>
+  </si>
+  <si>
+    <t>Integrate UI and Service</t>
+  </si>
+  <si>
+    <t>S5-109</t>
+  </si>
+  <si>
+    <t>Customer Onboarding Sanity Testing</t>
+  </si>
+  <si>
+    <t>S5-114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Test case for customer Agreement </t>
+  </si>
+  <si>
+    <t>S5-115</t>
+  </si>
+  <si>
+    <t>Sanity/Smoke Test Case for customer Agreement</t>
+  </si>
+  <si>
+    <t>S5-110</t>
+  </si>
+  <si>
+    <t>Configure EC2 Instance for Sales Service</t>
+  </si>
+  <si>
+    <t>S5-111</t>
+  </si>
+  <si>
+    <t>Test EC2 server for sales service webpage</t>
+  </si>
+  <si>
+    <t>Configure AWS CodeDeploy to deploy into EC2 Instance</t>
+  </si>
+  <si>
+    <t>S5-112</t>
+  </si>
+  <si>
+    <t>Test with AWS CodePipeline</t>
+  </si>
+  <si>
+    <t>S5-113</t>
+  </si>
+  <si>
+    <t>S5-104</t>
+  </si>
+  <si>
+    <t>Code: Database ORM in Node js</t>
+  </si>
+  <si>
+    <t>S5-105</t>
+  </si>
+  <si>
+    <t>Dev Test database integration</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Completion of Database Stories. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Few attributes for agreement view page related doubt cleared.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Commencement Sales Agreement View UI and API Development</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Discussion on CI/CD tool to be used. Decided to go with AWS Codepipeline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Demonstrated the service API working and Customer Onboarding UI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Discussed the functionality covered for both API and UI.</t>
+    </r>
+  </si>
+  <si>
+    <t>Standup 1 (03/10):</t>
+  </si>
+  <si>
+    <t>Standup 2 (03/21):</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cloud AWS CodePipeline configuration complete in AWS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Clarified on UI Design for Sales Onboarding page and as Team discussed few changes required.</t>
     </r>
   </si>
 </sst>
@@ -1373,7 +1652,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1474,6 +1753,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="70">
     <cellStyle name="Bad" xfId="67" builtinId="27"/>
@@ -1547,91 +1834,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="69" builtinId="25"/>
   </cellStyles>
-  <dxfs count="118">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="140">
     <dxf>
       <fill>
         <patternFill>
@@ -1702,20 +1905,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -1726,9 +1915,33 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1743,6 +1956,23 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C5700"/>
       </font>
@@ -1762,7 +1992,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1777,6 +2014,23 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C5700"/>
       </font>
@@ -1794,6 +2048,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -1821,13 +2089,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -1855,13 +2116,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -1889,13 +2143,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -1919,6 +2166,251 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2691,6 +3183,9 @@
                 <c:pt idx="1">
                   <c:v>43530</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>43551</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2705,6 +3200,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3316,6 +3814,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>54610</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Graphical user interface, line chart&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FA17789-1BDB-45B2-7084-80ACAAB46BB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8629650" y="152400"/>
+          <a:ext cx="2695575" cy="6277610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3708,7 +4255,7 @@
         <v>61</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>62</v>
@@ -3803,16 +4350,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.375" customWidth="1"/>
     <col min="3" max="3" width="255.625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3844,7 +4391,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3864,7 +4411,7 @@
         <v>91</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -3875,7 +4422,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -3886,7 +4433,7 @@
         <v>115</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -3897,7 +4444,7 @@
         <v>119</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3908,7 +4455,7 @@
         <v>118</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="F9" s="46"/>
     </row>
@@ -3930,204 +4477,236 @@
         <v>126</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="36"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>258</v>
-      </c>
+      <c r="B16" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="36"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>209</v>
+        <v>192</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>193</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>249</v>
+        <v>202</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="C26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B27" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="36"/>
-    </row>
-    <row r="25" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="32" t="s">
+      <c r="C27" s="36"/>
+    </row>
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="C26" s="45"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="9"/>
+      <c r="B30" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="45"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33"/>
     </row>
     <row r="34" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C34" s="9"/>
@@ -4155,92 +4734,44 @@
     </row>
     <row r="42" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C44" s="9"/>
+    </row>
+    <row r="45" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C45" s="9"/>
+    </row>
+    <row r="46" spans="3:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C46" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="4" priority="18" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="3" priority="17" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="EPIC-">
+  <conditionalFormatting sqref="A10:A18">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",A10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A12">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A11)))</formula>
+  <conditionalFormatting sqref="A20:A30">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:B18">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="EPIC-">
+  <conditionalFormatting sqref="A19:B19">
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",A19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A25">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4279,19 +4810,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4419,9 +4950,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
-        <v>3</v>
-      </c>
+      <c r="A9" s="16"/>
       <c r="B9" s="19" t="s">
         <v>113</v>
       </c>
@@ -4468,10 +4997,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>56</v>
@@ -4485,16 +5014,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>99</v>
+      <c r="E13" s="20" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4502,60 +5031,60 @@
         <v>2</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <v>3</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>286</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="32" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
-        <v>1</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>133</v>
-      </c>
+      <c r="C16" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>1</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="20" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4564,13 +5093,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>89</v>
+        <v>163</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>133</v>
@@ -4581,13 +5110,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>68</v>
+        <v>169</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>133</v>
@@ -4595,19 +5124,19 @@
     </row>
     <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>99</v>
+        <v>68</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -4615,33 +5144,33 @@
         <v>2</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
         <v>2</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>209</v>
+        <v>192</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>193</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -4649,373 +5178,437 @@
         <v>2</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D23" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="16">
+        <v>2</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E24" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
         <v>3</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="19" t="s">
+      <c r="B25" s="54" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
+        <v>3</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
+      <c r="B27" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="36"/>
+      <c r="E27" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
+        <v>3</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>278</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
+        <v>3</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="16"/>
+      <c r="B30" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
+        <v>2</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
-        <v>2</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="D27" s="19" t="s">
+      <c r="E31" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="55">
+        <v>3</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>293</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="19" t="s">
+      <c r="E32" s="19" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E3:E8 E24:E25 E28">
-    <cfRule type="containsText" dxfId="117" priority="85" operator="containsText" text="To Do">
+  <conditionalFormatting sqref="E3:E8 E27 E32">
+    <cfRule type="containsText" dxfId="139" priority="106" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="86" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="138" priority="107" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="87" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="137" priority="108" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="114" priority="70" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="136" priority="91" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="71" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="135" priority="92" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="72" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="134" priority="93" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="111" priority="69" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="133" priority="90" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsText" dxfId="110" priority="68" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="132" priority="89" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="109" priority="67" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="131" priority="88" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="108" priority="64" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="130" priority="85" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="65" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="129" priority="86" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="66" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="128" priority="87" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="containsText" dxfId="105" priority="63" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="127" priority="84" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="104" priority="60" operator="containsText" text="To Do">
+  <conditionalFormatting sqref="E12:E14">
+    <cfRule type="containsText" dxfId="126" priority="81" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="61" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="125" priority="82" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="62" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="124" priority="83" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsText" dxfId="123" priority="79" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="containsText" dxfId="122" priority="76" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="77" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="78" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="119" priority="75" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="containsText" dxfId="118" priority="72" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="73" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="74" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="containsText" dxfId="115" priority="71" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="containsText" dxfId="114" priority="68" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="113" priority="69" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="70" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:C19">
+    <cfRule type="containsText" dxfId="111" priority="67" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E24">
+    <cfRule type="containsText" dxfId="110" priority="64" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="65" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="66" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="107" priority="63" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="containsText" dxfId="103" priority="59" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="containsText" dxfId="99" priority="55" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="containsText" dxfId="92" priority="48" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="containsText" dxfId="88" priority="44" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="containsText" dxfId="84" priority="40" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="containsText" dxfId="80" priority="36" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="containsText" dxfId="76" priority="29" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="containsText" dxfId="75" priority="26" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="27" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="28" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="72" priority="25" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:E31">
+    <cfRule type="cellIs" dxfId="71" priority="22" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="23" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="24" operator="equal">
+      <formula>"To Do"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="68" priority="16" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="17" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="18" operator="equal">
+      <formula>"To Do"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="21" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="101" priority="58" operator="containsText" text="EPIC-">
+    <cfRule type="containsText" dxfId="62" priority="15" operator="containsText" text="EPIC-">
       <formula>NOT(ISERROR(SEARCH("EPIC-",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="100" priority="55" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",E16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="56" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",E16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="57" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",E16)))</formula>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="containsText" dxfId="61" priority="11" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="97" priority="54" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B16)))</formula>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="containsText" dxfId="60" priority="12" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="14" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="96" priority="51" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="52" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="53" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",E17)))</formula>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="containsText" dxfId="57" priority="7" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="93" priority="50" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B17)))</formula>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="containsText" dxfId="56" priority="8" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="9" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="10" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="containsText" dxfId="92" priority="47" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="48" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="49" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",E18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
-    <cfRule type="containsText" dxfId="89" priority="46" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="containsText" dxfId="88" priority="43" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",E19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="44" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",E19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="45" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",E19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="85" priority="42" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="containsText" dxfId="84" priority="39" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",E20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="40" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",E20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="41" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",E20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="81" priority="38" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="80" priority="35" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="36" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="37" operator="equal">
-      <formula>"To Do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="77" priority="34" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="containsText" dxfId="76" priority="31" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",E21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="32" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",E21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="33" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",E21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="73" priority="28" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="29" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="30" operator="equal">
-      <formula>"To Do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="70" priority="27" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="69" priority="24" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="25" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="26" operator="equal">
-      <formula>"To Do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="66" priority="23" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="65" priority="20" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="21" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="22" operator="equal">
-      <formula>"To Do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="62" priority="19" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="61" priority="16" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="17" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="18" operator="equal">
-      <formula>"To Do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="58" priority="15" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="57" priority="12" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="13" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="14" operator="equal">
-      <formula>"To Do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:B25">
-    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B24)))</formula>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",E25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",E25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",E26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",E26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",B26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
-      <formula>"To Do"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5219,17 +5812,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
     <col min="4" max="4" width="7.125" customWidth="1"/>
     <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
@@ -5285,6 +5878,27 @@
       <c r="F3" s="7">
         <f>(D3-D2)/E3*60</f>
         <v>74.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>43551</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>807</v>
+      </c>
+      <c r="E4">
+        <v>740</v>
+      </c>
+      <c r="F4" s="7">
+        <f>(D4-D3)/E4*60</f>
+        <v>53.351351351351354</v>
       </c>
     </row>
   </sheetData>
@@ -5311,8 +5925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A69" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5342,7 +5956,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>120</v>
@@ -5401,7 +6015,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>83</v>
       </c>
@@ -5420,7 +6034,7 @@
       <c r="H4" s="16"/>
       <c r="I4" s="28"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>84</v>
       </c>
@@ -5439,7 +6053,7 @@
       <c r="H5" s="16"/>
       <c r="I5" s="28"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>85</v>
       </c>
@@ -5458,7 +6072,7 @@
       <c r="H6" s="16"/>
       <c r="I6" s="28"/>
     </row>
-    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>86</v>
       </c>
@@ -5477,7 +6091,7 @@
       <c r="H7" s="16"/>
       <c r="I7" s="28"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>87</v>
       </c>
@@ -5971,10 +6585,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>56</v>
@@ -6032,7 +6646,7 @@
       <c r="H36" s="16"/>
       <c r="I36" s="28"/>
     </row>
-    <row r="37" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>136</v>
       </c>
@@ -6051,7 +6665,7 @@
       <c r="H37" s="16"/>
       <c r="I37" s="28"/>
     </row>
-    <row r="38" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>137</v>
       </c>
@@ -6075,7 +6689,7 @@
         <v>128</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C39" s="36"/>
       <c r="D39" s="36"/>
@@ -6087,10 +6701,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>68</v>
@@ -6116,10 +6730,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="27" t="s">
         <v>154</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>161</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>68</v>
@@ -6135,10 +6749,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>89</v>
@@ -6154,10 +6768,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>63</v>
@@ -6173,10 +6787,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>75</v>
@@ -6192,10 +6806,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C45" s="30" t="s">
         <v>63</v>
@@ -6221,10 +6835,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>63</v>
@@ -6240,10 +6854,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C47" s="29" t="s">
         <v>63</v>
@@ -6259,10 +6873,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C48" s="44" t="s">
         <v>89</v>
@@ -6288,10 +6902,10 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>89</v>
@@ -6307,10 +6921,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C50" s="19" t="s">
         <v>89</v>
@@ -6326,10 +6940,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>89</v>
@@ -6345,10 +6959,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C52" s="30" t="s">
         <v>68</v>
@@ -6375,10 +6989,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>68</v>
@@ -6395,10 +7009,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>75</v>
@@ -6451,13 +7065,13 @@
     </row>
     <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="39" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C59" s="40" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J59" s="2"/>
     </row>
@@ -6466,7 +7080,7 @@
         <v>133</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J60" s="2"/>
     </row>
@@ -6475,7 +7089,7 @@
         <v>92</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J61" s="2"/>
     </row>
@@ -6484,7 +7098,7 @@
         <v>99</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J62" s="2"/>
     </row>
@@ -6494,25 +7108,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B64" s="17" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="J64" s="2"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65" s="27" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="J65" s="2"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66" s="27" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="J66" s="2"/>
     </row>
     <row r="67" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B67" s="27" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="J67" s="2"/>
     </row>
@@ -6525,107 +7139,112 @@
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B70" s="17" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="J70" s="2"/>
     </row>
     <row r="71" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B71" s="52" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="J71" s="2"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B72" s="52" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="J72" s="2"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B73" s="52" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="J73" s="2"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B74" s="52" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="J74" s="2"/>
     </row>
     <row r="75" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B75" s="53" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B77" s="17" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B78" s="52" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B79" s="52" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B80" s="53" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B82" s="51" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B83" s="49" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B84" s="49" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B85" s="49" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B86" s="49" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B87" s="49" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="88" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B88" s="51" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B89" s="49" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B90" s="50" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E47:E54 D1:D54 D56:D1048576">
+  <conditionalFormatting sqref="A1:A1048576 B47:B48 B55 B57:B62">
+    <cfRule type="containsText" dxfId="47" priority="8" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D54 D56:D1048576 E47:E54">
     <cfRule type="containsText" dxfId="46" priority="9" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D1)))</formula>
     </cfRule>
@@ -6634,11 +7253,6 @@
     </cfRule>
     <cfRule type="containsText" dxfId="44" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47:B48 B55 B57:B62 A1:A1048576">
-    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6648,10 +7262,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A40" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6700,7 +7314,7 @@
         <v>128</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -6712,16 +7326,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>89</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="E3" s="25">
         <v>100</v>
@@ -6729,22 +7343,26 @@
       <c r="F3" s="25">
         <v>16</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="25">
+        <v>127</v>
+      </c>
+      <c r="H3" s="25">
+        <v>16</v>
+      </c>
       <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>89</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
@@ -6754,16 +7372,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>99</v>
+      <c r="D5" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -6773,16 +7391,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>99</v>
+      <c r="D6" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -6792,16 +7410,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>99</v>
+      <c r="D7" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -6811,16 +7429,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="E8" s="25">
         <v>100</v>
@@ -6828,22 +7446,26 @@
       <c r="F8" s="25">
         <v>16</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="G8" s="25">
+        <v>153</v>
+      </c>
+      <c r="H8" s="25">
+        <v>18</v>
+      </c>
       <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>99</v>
+      <c r="D9" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -6853,16 +7475,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>99</v>
+      <c r="D10" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -6872,16 +7494,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>99</v>
+      <c r="D11" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -6891,16 +7513,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E12" s="25">
         <v>150</v>
@@ -6908,22 +7530,26 @@
       <c r="F12" s="25">
         <v>16</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="G12" s="25">
+        <v>176</v>
+      </c>
+      <c r="H12" s="25">
+        <v>20</v>
+      </c>
       <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -6933,16 +7559,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -6952,16 +7578,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>99</v>
+      <c r="D15" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E15" s="25">
         <v>150</v>
@@ -6969,22 +7595,26 @@
       <c r="F15" s="25">
         <v>16</v>
       </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="G15" s="25">
+        <v>166</v>
+      </c>
+      <c r="H15" s="25">
+        <v>10</v>
+      </c>
       <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>99</v>
+      <c r="D16" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -6994,16 +7624,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>99</v>
+      <c r="D17" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -7019,7 +7649,9 @@
         <v>127</v>
       </c>
       <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+      <c r="D18" s="20" t="s">
+        <v>133</v>
+      </c>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
       <c r="G18" s="36"/>
@@ -7028,16 +7660,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>99</v>
+      <c r="D19" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E19" s="25">
         <v>100</v>
@@ -7045,22 +7677,26 @@
       <c r="F19" s="25">
         <v>16</v>
       </c>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="G19" s="25">
+        <v>106</v>
+      </c>
+      <c r="H19" s="25">
+        <v>10</v>
+      </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>99</v>
+      <c r="D20" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -7070,16 +7706,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>99</v>
+      <c r="D21" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E21" s="25">
         <v>40</v>
@@ -7087,22 +7723,26 @@
       <c r="F21" s="25">
         <v>16</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="G21" s="25">
+        <v>55</v>
+      </c>
+      <c r="H21" s="25">
+        <v>5</v>
+      </c>
       <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>99</v>
+      <c r="D22" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -7112,16 +7752,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>99</v>
+      <c r="D23" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -7134,10 +7774,12 @@
         <v>142</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
+      <c r="D24" s="20" t="s">
+        <v>133</v>
+      </c>
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
       <c r="G24" s="36"/>
@@ -7146,16 +7788,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>99</v>
+      <c r="D25" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E25" s="25">
         <v>100</v>
@@ -7163,22 +7805,26 @@
       <c r="F25" s="25">
         <v>24</v>
       </c>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
+      <c r="G25" s="25">
+        <v>24</v>
+      </c>
+      <c r="H25" s="25">
+        <v>10</v>
+      </c>
       <c r="I25" s="25"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>99</v>
+      <c r="D26" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -7188,16 +7834,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>99</v>
+      <c r="D27" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -7207,16 +7853,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>99</v>
+      <c r="D28" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -7226,16 +7872,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>99</v>
+      <c r="D29" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -7245,16 +7891,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>99</v>
+      <c r="D30" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -7273,118 +7919,262 @@
       </c>
       <c r="G31" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>807</v>
       </c>
       <c r="H31" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="17" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B41" s="57" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="57" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="57"/>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="57"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="52" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="52" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="53" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B54" s="52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B55" s="53" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="51" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B58" s="57" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B59" s="57" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B60" s="57" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="57" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="49"/>
+    </row>
+    <row r="63" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B63" s="51" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B64" s="57" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B65" s="57" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D3:D6">
-    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",D3)))</formula>
+  <conditionalFormatting sqref="A2:A24">
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A17 A19:A22">
-    <cfRule type="containsText" dxfId="39" priority="23" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A3)))</formula>
+  <conditionalFormatting sqref="D1:D32 D66:D1048576">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
+      <formula>"To Do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="To Do">
+  <conditionalFormatting sqref="D2:D30 D33:D65">
+    <cfRule type="containsText" dxfId="39" priority="20" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="38" priority="21" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="18" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="37" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="34" priority="18" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="31" priority="9" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="31" priority="15" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
-      <formula>"To Do"</formula>
+  <conditionalFormatting sqref="B33:B38">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I3"/>
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
@@ -7439,21 +8229,21 @@
       <c r="H2" s="36"/>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>113</v>
+        <v>278</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>144</v>
+        <v>280</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>99</v>
       </c>
       <c r="E3" s="25">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="F3" s="25">
         <v>16</v>
@@ -7462,15 +8252,15 @@
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>149</v>
+        <v>294</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>145</v>
+        <v>295</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>99</v>
@@ -7481,15 +8271,15 @@
       <c r="H4" s="16"/>
       <c r="I4" s="28"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>150</v>
+        <v>296</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>146</v>
+        <v>297</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>99</v>
@@ -7500,44 +8290,511 @@
       <c r="H5" s="16"/>
       <c r="I5" s="28"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="19" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="25">
+        <v>150</v>
+      </c>
+      <c r="F6" s="25">
+        <v>16</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="54" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="25">
+        <v>200</v>
+      </c>
+      <c r="F10" s="25">
+        <v>16</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>305</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="25">
+        <v>190</v>
+      </c>
+      <c r="F13" s="25">
+        <v>16</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="37"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D17" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="28"/>
+      <c r="E17" s="25">
+        <v>100</v>
+      </c>
+      <c r="F17" s="25">
+        <v>24</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="25">
+        <v>100</v>
+      </c>
+      <c r="F23" s="25">
+        <v>16</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="54" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16">
+        <f>SUM(E3:E25)</f>
+        <v>890</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" ref="F26:H26" si="0">SUM(F3:F25)</f>
+        <v>104</v>
+      </c>
+      <c r="G26" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D6">
-    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="To Do">
+  <conditionalFormatting sqref="A2:A8">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D8 D10:D15">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A6">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="EPIC-">
-      <formula>NOT(ISERROR(SEARCH("EPIC-",A2)))</formula>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+      <formula>"To Do"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",D9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="26" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",D9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D25">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>"To Do"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D25">
+    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="19" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="20" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:A23">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="EPIC-">
+      <formula>NOT(ISERROR(SEARCH("EPIC-",A22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>